<commit_message>
Updated demo data dictionary
</commit_message>
<xml_diff>
--- a/Demo Data Dictionary.xlsx
+++ b/Demo Data Dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\deyta-userguide\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E2610E2-885A-4B3A-9599-8D75478B93FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28694237-661A-4590-A602-55242A0E26F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-5700" windowWidth="38620" windowHeight="21100" firstSheet="2" activeTab="7" xr2:uid="{F65A8243-5860-4D99-919D-391CF520B627}"/>
+    <workbookView xWindow="-38510" yWindow="-5700" windowWidth="38620" windowHeight="21100" firstSheet="2" activeTab="2" xr2:uid="{F65A8243-5860-4D99-919D-391CF520B627}"/>
   </bookViews>
   <sheets>
     <sheet name="Explanatory Note" sheetId="1" r:id="rId1"/>
@@ -924,9 +924,6 @@
     <t>Green</t>
   </si>
   <si>
-    <t>#00FF00</t>
-  </si>
-  <si>
     <t>Oversees customer data, loyalty programs, and feedback</t>
   </si>
   <si>
@@ -1954,6 +1951,9 @@
   </si>
   <si>
     <t>["scheduled_movies", "director", "release_date", "genre", "theater"]</t>
+  </si>
+  <si>
+    <t>#006400</t>
   </si>
 </sst>
 </file>
@@ -2699,7 +2699,7 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>453390</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>120780</xdr:rowOff>
+      <xdr:rowOff>116970</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3229,10 +3229,10 @@
         <v>40</v>
       </c>
       <c r="B1" s="51" t="s">
+        <v>500</v>
+      </c>
+      <c r="C1" s="51" t="s">
         <v>501</v>
-      </c>
-      <c r="C1" s="51" t="s">
-        <v>502</v>
       </c>
       <c r="D1" s="51" t="s">
         <v>251</v>
@@ -3252,1380 +3252,1380 @@
     </row>
     <row r="2" spans="1:8" ht="14.4" thickBot="1">
       <c r="A2" s="50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B2" s="50" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C2" s="50" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D2" s="50" t="s">
+        <v>428</v>
+      </c>
+      <c r="E2" s="50" t="s">
+        <v>384</v>
+      </c>
+      <c r="F2" s="50" t="s">
         <v>429</v>
       </c>
-      <c r="E2" s="50" t="s">
-        <v>385</v>
-      </c>
-      <c r="F2" s="50" t="s">
-        <v>430</v>
-      </c>
       <c r="G2" s="50" t="s">
+        <v>386</v>
+      </c>
+      <c r="H2" s="50" t="s">
         <v>387</v>
-      </c>
-      <c r="H2" s="50" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="14.4" thickBot="1">
       <c r="A3" s="50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B3" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C3" s="44" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D3" s="44" t="s">
+        <v>433</v>
+      </c>
+      <c r="E3" s="44" t="s">
+        <v>384</v>
+      </c>
+      <c r="F3" s="44" t="s">
         <v>434</v>
       </c>
-      <c r="E3" s="44" t="s">
-        <v>385</v>
-      </c>
-      <c r="F3" s="44" t="s">
+      <c r="G3" s="44" t="s">
         <v>435</v>
       </c>
-      <c r="G3" s="44" t="s">
-        <v>436</v>
-      </c>
       <c r="H3" s="44" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="14.4" thickBot="1">
       <c r="A4" s="50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B4" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C4" s="44" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D4" s="44" t="s">
+        <v>430</v>
+      </c>
+      <c r="E4" s="44" t="s">
+        <v>509</v>
+      </c>
+      <c r="F4" s="44" t="s">
         <v>431</v>
       </c>
-      <c r="E4" s="44" t="s">
-        <v>510</v>
-      </c>
-      <c r="F4" s="44" t="s">
+      <c r="G4" s="44" t="s">
         <v>432</v>
       </c>
-      <c r="G4" s="44" t="s">
-        <v>433</v>
-      </c>
       <c r="H4" s="44" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="14.4" thickBot="1">
       <c r="A5" s="50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B5" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C5" s="44" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D5" s="44" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E5" s="44" t="s">
         <v>91</v>
       </c>
       <c r="F5" s="44" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="G5" s="44" t="s">
+        <v>390</v>
+      </c>
+      <c r="H5" s="44" t="s">
         <v>391</v>
-      </c>
-      <c r="H5" s="44" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="14.4" thickBot="1">
       <c r="A6" s="50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B6" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C6" s="44" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D6" s="44" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E6" s="44" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F6" s="44" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="G6" s="44" t="s">
+        <v>386</v>
+      </c>
+      <c r="H6" s="44" t="s">
         <v>387</v>
-      </c>
-      <c r="H6" s="44" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="14.4" thickBot="1">
       <c r="A7" s="50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B7" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D7" s="44" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E7" s="44" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="F7" s="44" t="s">
+        <v>424</v>
+      </c>
+      <c r="G7" s="44" t="s">
         <v>425</v>
       </c>
-      <c r="G7" s="44" t="s">
-        <v>426</v>
-      </c>
       <c r="H7" s="44" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="14.4" thickBot="1">
       <c r="A8" s="50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B8" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C8" s="44" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D8" s="44" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E8" s="44" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F8" s="44" t="s">
+        <v>418</v>
+      </c>
+      <c r="G8" s="44" t="s">
         <v>419</v>
       </c>
-      <c r="G8" s="44" t="s">
-        <v>420</v>
-      </c>
       <c r="H8" s="44" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="14.4" thickBot="1">
       <c r="A9" s="50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B9" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C9" s="44" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D9" s="44" t="s">
+        <v>420</v>
+      </c>
+      <c r="E9" s="44" t="s">
+        <v>508</v>
+      </c>
+      <c r="F9" s="44" t="s">
         <v>421</v>
       </c>
-      <c r="E9" s="44" t="s">
-        <v>509</v>
-      </c>
-      <c r="F9" s="44" t="s">
-        <v>422</v>
-      </c>
       <c r="G9" s="44" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H9" s="44" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="14.4" thickBot="1">
       <c r="A10" s="50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B10" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C10" s="44" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D10" s="44" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E10" s="44" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F10" s="44" t="s">
+        <v>474</v>
+      </c>
+      <c r="G10" s="44" t="s">
         <v>475</v>
       </c>
-      <c r="G10" s="44" t="s">
-        <v>476</v>
-      </c>
       <c r="H10" s="44" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="14.4" thickBot="1">
       <c r="A11" s="50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B11" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C11" s="44" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D11" s="44" t="s">
+        <v>479</v>
+      </c>
+      <c r="E11" s="44" t="s">
+        <v>384</v>
+      </c>
+      <c r="F11" s="44" t="s">
         <v>480</v>
       </c>
-      <c r="E11" s="44" t="s">
-        <v>385</v>
-      </c>
-      <c r="F11" s="44" t="s">
-        <v>481</v>
-      </c>
       <c r="G11" s="44" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="H11" s="44" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="14.4" thickBot="1">
       <c r="A12" s="50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B12" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C12" s="44" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D12" s="44" t="s">
+        <v>476</v>
+      </c>
+      <c r="E12" s="44" t="s">
+        <v>508</v>
+      </c>
+      <c r="F12" s="44" t="s">
         <v>477</v>
       </c>
-      <c r="E12" s="44" t="s">
-        <v>509</v>
-      </c>
-      <c r="F12" s="44" t="s">
+      <c r="G12" s="44" t="s">
         <v>478</v>
       </c>
-      <c r="G12" s="44" t="s">
-        <v>479</v>
-      </c>
       <c r="H12" s="44" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="14.4" thickBot="1">
       <c r="A13" s="50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B13" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C13" s="44" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D13" s="44" t="s">
+        <v>472</v>
+      </c>
+      <c r="E13" s="44" t="s">
+        <v>384</v>
+      </c>
+      <c r="F13" s="44" t="s">
         <v>473</v>
       </c>
-      <c r="E13" s="44" t="s">
-        <v>385</v>
-      </c>
-      <c r="F13" s="44" t="s">
-        <v>474</v>
-      </c>
       <c r="G13" s="44" t="s">
+        <v>386</v>
+      </c>
+      <c r="H13" s="44" t="s">
         <v>387</v>
-      </c>
-      <c r="H13" s="44" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="14.4" thickBot="1">
       <c r="A14" s="50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B14" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C14" s="44" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D14" s="44" t="s">
+        <v>438</v>
+      </c>
+      <c r="E14" s="44" t="s">
+        <v>384</v>
+      </c>
+      <c r="F14" s="44" t="s">
         <v>439</v>
       </c>
-      <c r="E14" s="44" t="s">
-        <v>385</v>
-      </c>
-      <c r="F14" s="44" t="s">
+      <c r="G14" s="44" t="s">
         <v>440</v>
       </c>
-      <c r="G14" s="44" t="s">
-        <v>441</v>
-      </c>
       <c r="H14" s="44" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="14.4" thickBot="1">
       <c r="A15" s="50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B15" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C15" s="44" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D15" s="44" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E15" s="44" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F15" s="44" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="G15" s="44" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="H15" s="44" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="14.4" thickBot="1">
       <c r="A16" s="50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B16" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C16" s="44" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D16" s="44" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E16" s="44" t="s">
         <v>91</v>
       </c>
       <c r="F16" s="44" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G16" s="44" t="s">
+        <v>390</v>
+      </c>
+      <c r="H16" s="44" t="s">
         <v>391</v>
-      </c>
-      <c r="H16" s="44" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="14.4" thickBot="1">
       <c r="A17" s="50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B17" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C17" s="44" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D17" s="44" t="s">
+        <v>383</v>
+      </c>
+      <c r="E17" s="44" t="s">
         <v>384</v>
       </c>
-      <c r="E17" s="44" t="s">
-        <v>385</v>
-      </c>
       <c r="F17" s="44" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G17" s="44" t="s">
+        <v>386</v>
+      </c>
+      <c r="H17" s="44" t="s">
         <v>387</v>
-      </c>
-      <c r="H17" s="44" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="14.4" thickBot="1">
       <c r="A18" s="50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B18" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C18" s="44" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D18" s="44" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E18" s="44" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F18" s="44" t="s">
+        <v>403</v>
+      </c>
+      <c r="G18" s="44" t="s">
         <v>404</v>
       </c>
-      <c r="G18" s="44" t="s">
-        <v>405</v>
-      </c>
       <c r="H18" s="44" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="14.4" thickBot="1">
       <c r="A19" s="50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B19" s="44" t="s">
+        <v>295</v>
+      </c>
+      <c r="C19" s="44" t="s">
         <v>296</v>
       </c>
-      <c r="C19" s="44" t="s">
-        <v>297</v>
-      </c>
       <c r="D19" s="44" t="s">
+        <v>392</v>
+      </c>
+      <c r="E19" s="44" t="s">
+        <v>384</v>
+      </c>
+      <c r="F19" s="44" t="s">
         <v>393</v>
       </c>
-      <c r="E19" s="44" t="s">
-        <v>385</v>
-      </c>
-      <c r="F19" s="44" t="s">
+      <c r="G19" s="44" t="s">
         <v>394</v>
       </c>
-      <c r="G19" s="44" t="s">
-        <v>395</v>
-      </c>
       <c r="H19" s="44" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="14.4" thickBot="1">
       <c r="A20" s="50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B20" s="44" t="s">
+        <v>295</v>
+      </c>
+      <c r="C20" s="44" t="s">
         <v>296</v>
       </c>
-      <c r="C20" s="44" t="s">
-        <v>297</v>
-      </c>
       <c r="D20" s="44" t="s">
+        <v>395</v>
+      </c>
+      <c r="E20" s="44" t="s">
+        <v>384</v>
+      </c>
+      <c r="F20" s="44" t="s">
         <v>396</v>
       </c>
-      <c r="E20" s="44" t="s">
-        <v>385</v>
-      </c>
-      <c r="F20" s="44" t="s">
+      <c r="G20" s="44" t="s">
         <v>397</v>
       </c>
-      <c r="G20" s="44" t="s">
-        <v>398</v>
-      </c>
       <c r="H20" s="44" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="14.4" thickBot="1">
       <c r="A21" s="50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B21" s="44" t="s">
+        <v>295</v>
+      </c>
+      <c r="C21" s="44" t="s">
         <v>296</v>
       </c>
-      <c r="C21" s="44" t="s">
-        <v>297</v>
-      </c>
       <c r="D21" s="44" t="s">
+        <v>398</v>
+      </c>
+      <c r="E21" s="44" t="s">
+        <v>384</v>
+      </c>
+      <c r="F21" s="44" t="s">
         <v>399</v>
       </c>
-      <c r="E21" s="44" t="s">
-        <v>385</v>
-      </c>
-      <c r="F21" s="44" t="s">
+      <c r="G21" s="44" t="s">
         <v>400</v>
       </c>
-      <c r="G21" s="44" t="s">
-        <v>401</v>
-      </c>
       <c r="H21" s="44" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="14.4" thickBot="1">
       <c r="A22" s="50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B22" s="44" t="s">
+        <v>295</v>
+      </c>
+      <c r="C22" s="44" t="s">
         <v>296</v>
       </c>
-      <c r="C22" s="44" t="s">
-        <v>297</v>
-      </c>
       <c r="D22" s="44" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E22" s="44" t="s">
         <v>91</v>
       </c>
       <c r="F22" s="44" t="s">
+        <v>389</v>
+      </c>
+      <c r="G22" s="44" t="s">
         <v>390</v>
       </c>
-      <c r="G22" s="44" t="s">
+      <c r="H22" s="44" t="s">
         <v>391</v>
-      </c>
-      <c r="H22" s="44" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="14.4" thickBot="1">
       <c r="A23" s="50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B23" s="44" t="s">
+        <v>295</v>
+      </c>
+      <c r="C23" s="44" t="s">
         <v>296</v>
       </c>
-      <c r="C23" s="44" t="s">
-        <v>297</v>
-      </c>
       <c r="D23" s="44" t="s">
+        <v>383</v>
+      </c>
+      <c r="E23" s="44" t="s">
         <v>384</v>
       </c>
-      <c r="E23" s="44" t="s">
+      <c r="F23" s="44" t="s">
         <v>385</v>
       </c>
-      <c r="F23" s="44" t="s">
+      <c r="G23" s="44" t="s">
         <v>386</v>
       </c>
-      <c r="G23" s="44" t="s">
+      <c r="H23" s="44" t="s">
         <v>387</v>
-      </c>
-      <c r="H23" s="44" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="14.4" thickBot="1">
       <c r="A24" s="50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B24" s="44" t="s">
+        <v>295</v>
+      </c>
+      <c r="C24" s="44" t="s">
         <v>296</v>
       </c>
-      <c r="C24" s="44" t="s">
-        <v>297</v>
-      </c>
       <c r="D24" s="44" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E24" s="44" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F24" s="44" t="s">
+        <v>403</v>
+      </c>
+      <c r="G24" s="44" t="s">
         <v>404</v>
       </c>
-      <c r="G24" s="44" t="s">
-        <v>405</v>
-      </c>
       <c r="H24" s="44" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="14.4" thickBot="1">
       <c r="A25" s="50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B25" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C25" s="44" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D25" s="44" t="s">
+        <v>461</v>
+      </c>
+      <c r="E25" s="44" t="s">
+        <v>384</v>
+      </c>
+      <c r="F25" s="44" t="s">
         <v>462</v>
       </c>
-      <c r="E25" s="44" t="s">
-        <v>385</v>
-      </c>
-      <c r="F25" s="44" t="s">
-        <v>463</v>
-      </c>
       <c r="G25" s="44" t="s">
+        <v>386</v>
+      </c>
+      <c r="H25" s="44" t="s">
         <v>387</v>
-      </c>
-      <c r="H25" s="44" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="14.4" thickBot="1">
       <c r="A26" s="50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B26" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C26" s="44" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D26" s="44" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E26" s="44" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F26" s="44" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="G26" s="44" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H26" s="44" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="14.4" thickBot="1">
       <c r="A27" s="50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B27" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C27" s="44" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D27" s="44" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E27" s="44" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F27" s="44" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="G27" s="44" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H27" s="44" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="14.4" thickBot="1">
       <c r="A28" s="50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B28" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C28" s="44" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D28" s="44" t="s">
+        <v>468</v>
+      </c>
+      <c r="E28" s="44" t="s">
+        <v>384</v>
+      </c>
+      <c r="F28" s="44" t="s">
         <v>469</v>
       </c>
-      <c r="E28" s="44" t="s">
-        <v>385</v>
-      </c>
-      <c r="F28" s="44" t="s">
-        <v>470</v>
-      </c>
       <c r="G28" s="44" t="s">
+        <v>386</v>
+      </c>
+      <c r="H28" s="44" t="s">
         <v>387</v>
-      </c>
-      <c r="H28" s="44" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="14.4" thickBot="1">
       <c r="A29" s="50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B29" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C29" s="44" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D29" s="44" t="s">
+        <v>470</v>
+      </c>
+      <c r="E29" s="44" t="s">
+        <v>508</v>
+      </c>
+      <c r="F29" s="44" t="s">
         <v>471</v>
       </c>
-      <c r="E29" s="44" t="s">
-        <v>509</v>
-      </c>
-      <c r="F29" s="44" t="s">
-        <v>472</v>
-      </c>
       <c r="G29" s="44" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="H29" s="44" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="14.4" thickBot="1">
       <c r="A30" s="50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B30" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C30" s="44" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D30" s="44" t="s">
+        <v>485</v>
+      </c>
+      <c r="E30" s="44" t="s">
+        <v>384</v>
+      </c>
+      <c r="F30" s="44" t="s">
         <v>486</v>
       </c>
-      <c r="E30" s="44" t="s">
-        <v>385</v>
-      </c>
-      <c r="F30" s="44" t="s">
-        <v>487</v>
-      </c>
       <c r="G30" s="44" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H30" s="44" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="14.4" thickBot="1">
       <c r="A31" s="50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B31" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C31" s="44" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D31" s="44" t="s">
+        <v>481</v>
+      </c>
+      <c r="E31" s="44" t="s">
+        <v>384</v>
+      </c>
+      <c r="F31" s="44" t="s">
         <v>482</v>
       </c>
-      <c r="E31" s="44" t="s">
-        <v>385</v>
-      </c>
-      <c r="F31" s="44" t="s">
-        <v>483</v>
-      </c>
       <c r="G31" s="44" t="s">
+        <v>386</v>
+      </c>
+      <c r="H31" s="44" t="s">
         <v>387</v>
-      </c>
-      <c r="H31" s="44" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="14.4" thickBot="1">
       <c r="A32" s="50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B32" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C32" s="44" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D32" s="44" t="s">
+        <v>483</v>
+      </c>
+      <c r="E32" s="44" t="s">
+        <v>509</v>
+      </c>
+      <c r="F32" s="44" t="s">
         <v>484</v>
       </c>
-      <c r="E32" s="44" t="s">
-        <v>510</v>
-      </c>
-      <c r="F32" s="44" t="s">
-        <v>485</v>
-      </c>
       <c r="G32" s="44" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="H32" s="44" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="14.4" thickBot="1">
       <c r="A33" s="50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B33" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C33" s="44" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D33" s="44" t="s">
+        <v>446</v>
+      </c>
+      <c r="E33" s="44" t="s">
+        <v>508</v>
+      </c>
+      <c r="F33" s="44" t="s">
         <v>447</v>
       </c>
-      <c r="E33" s="44" t="s">
-        <v>509</v>
-      </c>
-      <c r="F33" s="44" t="s">
+      <c r="G33" s="44" t="s">
         <v>448</v>
       </c>
-      <c r="G33" s="44" t="s">
-        <v>449</v>
-      </c>
       <c r="H33" s="44" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="14.4" thickBot="1">
       <c r="A34" s="50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B34" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C34" s="44" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D34" s="44" t="s">
         <v>69</v>
       </c>
       <c r="E34" s="44" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F34" s="44" t="s">
+        <v>449</v>
+      </c>
+      <c r="G34" s="44" t="s">
         <v>450</v>
       </c>
-      <c r="G34" s="44" t="s">
-        <v>451</v>
-      </c>
       <c r="H34" s="44" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="14.4" thickBot="1">
       <c r="A35" s="50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B35" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C35" s="44" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D35" s="44" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E35" s="44" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F35" s="44" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="G35" s="44" t="s">
+        <v>386</v>
+      </c>
+      <c r="H35" s="44" t="s">
         <v>387</v>
-      </c>
-      <c r="H35" s="44" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="14.4" thickBot="1">
       <c r="A36" s="50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B36" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C36" s="44" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D36" s="44" t="s">
+        <v>443</v>
+      </c>
+      <c r="E36" s="44" t="s">
+        <v>509</v>
+      </c>
+      <c r="F36" s="44" t="s">
         <v>444</v>
       </c>
-      <c r="E36" s="44" t="s">
-        <v>510</v>
-      </c>
-      <c r="F36" s="44" t="s">
+      <c r="G36" s="44" t="s">
         <v>445</v>
       </c>
-      <c r="G36" s="44" t="s">
-        <v>446</v>
-      </c>
       <c r="H36" s="44" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="14.4" thickBot="1">
       <c r="A37" s="50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B37" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C37" s="44" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D37" s="44" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E37" s="44" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F37" s="44" t="s">
+        <v>453</v>
+      </c>
+      <c r="G37" s="44" t="s">
         <v>454</v>
       </c>
-      <c r="G37" s="44" t="s">
-        <v>455</v>
-      </c>
       <c r="H37" s="44" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="14.4" thickBot="1">
       <c r="A38" s="50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B38" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C38" s="44" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D38" s="44" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E38" s="44" t="s">
         <v>91</v>
       </c>
       <c r="F38" s="44" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G38" s="44" t="s">
+        <v>390</v>
+      </c>
+      <c r="H38" s="44" t="s">
         <v>391</v>
-      </c>
-      <c r="H38" s="44" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="14.4" thickBot="1">
       <c r="A39" s="50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B39" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C39" s="44" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D39" s="44" t="s">
+        <v>465</v>
+      </c>
+      <c r="E39" s="44" t="s">
+        <v>384</v>
+      </c>
+      <c r="F39" s="44" t="s">
         <v>466</v>
       </c>
-      <c r="E39" s="44" t="s">
-        <v>385</v>
-      </c>
-      <c r="F39" s="44" t="s">
-        <v>467</v>
-      </c>
       <c r="G39" s="44" t="s">
+        <v>386</v>
+      </c>
+      <c r="H39" s="44" t="s">
         <v>387</v>
-      </c>
-      <c r="H39" s="44" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="14.4" thickBot="1">
       <c r="A40" s="50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B40" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C40" s="44" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D40" s="44" t="s">
+        <v>405</v>
+      </c>
+      <c r="E40" s="44" t="s">
+        <v>384</v>
+      </c>
+      <c r="F40" s="44" t="s">
         <v>406</v>
       </c>
-      <c r="E40" s="44" t="s">
-        <v>385</v>
-      </c>
-      <c r="F40" s="44" t="s">
-        <v>407</v>
-      </c>
       <c r="G40" s="44" t="s">
+        <v>386</v>
+      </c>
+      <c r="H40" s="44" t="s">
         <v>387</v>
-      </c>
-      <c r="H40" s="44" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="14.4" thickBot="1">
       <c r="A41" s="50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B41" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C41" s="44" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D41" s="44" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E41" s="44" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F41" s="44" t="s">
+        <v>411</v>
+      </c>
+      <c r="G41" s="44" t="s">
         <v>412</v>
       </c>
-      <c r="G41" s="44" t="s">
-        <v>413</v>
-      </c>
       <c r="H41" s="44" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="14.4" thickBot="1">
       <c r="A42" s="50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B42" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C42" s="44" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D42" s="44" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E42" s="44" t="s">
         <v>91</v>
       </c>
       <c r="F42" s="44" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="G42" s="44" t="s">
+        <v>390</v>
+      </c>
+      <c r="H42" s="44" t="s">
         <v>391</v>
-      </c>
-      <c r="H42" s="44" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="14.4" thickBot="1">
       <c r="A43" s="50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B43" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C43" s="44" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D43" s="44" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E43" s="44" t="s">
         <v>65</v>
       </c>
       <c r="F43" s="44" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G43" s="44" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="H43" s="44" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="14.4" thickBot="1">
       <c r="A44" s="50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B44" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C44" s="44" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D44" s="44" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E44" s="44" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F44" s="44" t="s">
+        <v>453</v>
+      </c>
+      <c r="G44" s="44" t="s">
         <v>454</v>
       </c>
-      <c r="G44" s="44" t="s">
-        <v>455</v>
-      </c>
       <c r="H44" s="44" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="14.4" thickBot="1">
       <c r="A45" s="50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B45" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C45" s="44" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D45" s="44" t="s">
+        <v>451</v>
+      </c>
+      <c r="E45" s="44" t="s">
+        <v>384</v>
+      </c>
+      <c r="F45" s="44" t="s">
         <v>452</v>
       </c>
-      <c r="E45" s="44" t="s">
-        <v>385</v>
-      </c>
-      <c r="F45" s="44" t="s">
-        <v>453</v>
-      </c>
       <c r="G45" s="44" t="s">
+        <v>386</v>
+      </c>
+      <c r="H45" s="44" t="s">
         <v>387</v>
-      </c>
-      <c r="H45" s="44" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="14.4" thickBot="1">
       <c r="A46" s="50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B46" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C46" s="44" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D46" s="44" t="s">
+        <v>458</v>
+      </c>
+      <c r="E46" s="44" t="s">
         <v>459</v>
       </c>
-      <c r="E46" s="44" t="s">
+      <c r="F46" s="44" t="s">
         <v>460</v>
       </c>
-      <c r="F46" s="44" t="s">
-        <v>461</v>
-      </c>
       <c r="G46" s="44" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="H46" s="44" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="14.4" thickBot="1">
       <c r="A47" s="50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B47" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C47" s="44" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D47" s="44" t="s">
+        <v>455</v>
+      </c>
+      <c r="E47" s="44" t="s">
+        <v>384</v>
+      </c>
+      <c r="F47" s="44" t="s">
         <v>456</v>
       </c>
-      <c r="E47" s="44" t="s">
-        <v>385</v>
-      </c>
-      <c r="F47" s="44" t="s">
+      <c r="G47" s="44" t="s">
         <v>457</v>
       </c>
-      <c r="G47" s="44" t="s">
-        <v>458</v>
-      </c>
       <c r="H47" s="44" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="14.4" thickBot="1">
       <c r="A48" s="50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B48" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C48" s="44" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D48" s="44" t="s">
+        <v>488</v>
+      </c>
+      <c r="E48" s="44" t="s">
+        <v>384</v>
+      </c>
+      <c r="F48" s="44" t="s">
         <v>489</v>
       </c>
-      <c r="E48" s="44" t="s">
-        <v>385</v>
-      </c>
-      <c r="F48" s="44" t="s">
+      <c r="G48" s="44" t="s">
         <v>490</v>
       </c>
-      <c r="G48" s="44" t="s">
-        <v>491</v>
-      </c>
       <c r="H48" s="44" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="14.4" thickBot="1">
       <c r="A49" s="50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B49" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C49" s="44" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D49" s="44" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="E49" s="44" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F49" s="44" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="G49" s="44" t="s">
+        <v>386</v>
+      </c>
+      <c r="H49" s="44" t="s">
         <v>387</v>
-      </c>
-      <c r="H49" s="44" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="14.4" thickBot="1">
       <c r="A50" s="50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B50" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C50" s="44" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D50" s="44" t="s">
+        <v>493</v>
+      </c>
+      <c r="E50" s="44" t="s">
+        <v>459</v>
+      </c>
+      <c r="F50" s="44" t="s">
         <v>494</v>
       </c>
-      <c r="E50" s="44" t="s">
-        <v>460</v>
-      </c>
-      <c r="F50" s="44" t="s">
-        <v>495</v>
-      </c>
       <c r="G50" s="44" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="H50" s="44" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="14.4" thickBot="1">
       <c r="A51" s="50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B51" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C51" s="44" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D51" s="44" t="s">
+        <v>491</v>
+      </c>
+      <c r="E51" s="44" t="s">
+        <v>459</v>
+      </c>
+      <c r="F51" s="44" t="s">
         <v>492</v>
       </c>
-      <c r="E51" s="44" t="s">
-        <v>460</v>
-      </c>
-      <c r="F51" s="44" t="s">
-        <v>493</v>
-      </c>
       <c r="G51" s="44" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="H51" s="44" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="14.4" thickBot="1">
       <c r="A52" s="50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B52" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C52" s="44" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D52" s="44" t="s">
+        <v>498</v>
+      </c>
+      <c r="E52" s="44" t="s">
+        <v>384</v>
+      </c>
+      <c r="F52" s="44" t="s">
         <v>499</v>
       </c>
-      <c r="E52" s="44" t="s">
-        <v>385</v>
-      </c>
-      <c r="F52" s="44" t="s">
-        <v>500</v>
-      </c>
       <c r="G52" s="44" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H52" s="44" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="14.4" thickBot="1">
       <c r="A53" s="50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B53" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C53" s="44" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D53" s="44" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="E53" s="44" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F53" s="44" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="G53" s="44" t="s">
+        <v>386</v>
+      </c>
+      <c r="H53" s="44" t="s">
         <v>387</v>
-      </c>
-      <c r="H53" s="44" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="14.4" thickBot="1">
       <c r="A54" s="50" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B54" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C54" s="44" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D54" s="44" t="s">
+        <v>496</v>
+      </c>
+      <c r="E54" s="44" t="s">
+        <v>509</v>
+      </c>
+      <c r="F54" s="44" t="s">
         <v>497</v>
       </c>
-      <c r="E54" s="44" t="s">
-        <v>510</v>
-      </c>
-      <c r="F54" s="44" t="s">
-        <v>498</v>
-      </c>
       <c r="G54" s="44" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="H54" s="44" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
   </sheetData>
@@ -7394,8 +7394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC6DFD0C-45CD-4C4B-8F90-D9F3057A9BEA}">
   <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView zoomScale="196" zoomScaleNormal="196" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" zoomScale="196" zoomScaleNormal="196" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -7429,7 +7429,7 @@
         <v>32</v>
       </c>
       <c r="F1" s="33" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="G1" s="33" t="s">
         <v>33</v>
@@ -7548,25 +7548,25 @@
         <v>278</v>
       </c>
       <c r="C5" s="31" t="s">
+        <v>622</v>
+      </c>
+      <c r="D5" s="31" t="s">
         <v>279</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="E5" s="31" t="s">
         <v>280</v>
       </c>
-      <c r="E5" s="31" t="s">
+      <c r="F5" s="31" t="s">
         <v>281</v>
       </c>
-      <c r="F5" s="31" t="s">
+      <c r="G5" s="31" t="s">
         <v>282</v>
       </c>
-      <c r="G5" s="31" t="s">
+      <c r="H5" s="31" t="s">
         <v>283</v>
       </c>
-      <c r="H5" s="31" t="s">
+      <c r="I5" s="31" t="s">
         <v>284</v>
-      </c>
-      <c r="I5" s="31" t="s">
-        <v>285</v>
       </c>
       <c r="J5" s="31" t="s">
         <v>259</v>
@@ -7574,31 +7574,31 @@
     </row>
     <row r="6" spans="1:10" ht="28.2" thickBot="1">
       <c r="A6" s="31" t="s">
+        <v>285</v>
+      </c>
+      <c r="B6" s="31" t="s">
         <v>286</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="C6" s="31" t="s">
         <v>287</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="D6" s="31" t="s">
         <v>288</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="E6" s="31" t="s">
         <v>289</v>
       </c>
-      <c r="E6" s="31" t="s">
+      <c r="F6" s="31" t="s">
         <v>290</v>
       </c>
-      <c r="F6" s="31" t="s">
+      <c r="G6" s="31" t="s">
         <v>291</v>
       </c>
-      <c r="G6" s="31" t="s">
+      <c r="H6" s="31" t="s">
         <v>292</v>
       </c>
-      <c r="H6" s="31" t="s">
+      <c r="I6" s="31" t="s">
         <v>293</v>
-      </c>
-      <c r="I6" s="31" t="s">
-        <v>294</v>
       </c>
       <c r="J6" s="31" t="s">
         <v>259</v>
@@ -7874,10 +7874,10 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B2" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
   </sheetData>
@@ -7909,10 +7909,10 @@
     </row>
     <row r="2" spans="1:2" ht="15" thickBot="1">
       <c r="A2" s="44" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B2" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
   </sheetData>
@@ -7955,13 +7955,13 @@
         <v>40</v>
       </c>
       <c r="C1" s="33" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D1" s="33" t="s">
         <v>251</v>
       </c>
       <c r="E1" s="33" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F1" s="46" t="s">
         <v>41</v>
@@ -7996,43 +7996,43 @@
         <v>252</v>
       </c>
       <c r="B2" s="44" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C2" s="44" t="s">
+        <v>295</v>
+      </c>
+      <c r="D2" s="44" t="s">
         <v>296</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="E2" s="44" t="s">
+        <v>505</v>
+      </c>
+      <c r="F2" s="44" t="s">
         <v>297</v>
       </c>
-      <c r="E2" s="44" t="s">
-        <v>506</v>
-      </c>
-      <c r="F2" s="44" t="s">
+      <c r="G2" s="44" t="s">
         <v>298</v>
       </c>
-      <c r="G2" s="44" t="s">
+      <c r="H2" s="44" t="s">
+        <v>297</v>
+      </c>
+      <c r="I2" s="44" t="s">
         <v>299</v>
       </c>
-      <c r="H2" s="44" t="s">
-        <v>298</v>
-      </c>
-      <c r="I2" s="44" t="s">
+      <c r="J2" s="44" t="s">
         <v>300</v>
       </c>
-      <c r="J2" s="44" t="s">
+      <c r="K2" s="44" t="s">
         <v>301</v>
       </c>
-      <c r="K2" s="44" t="s">
+      <c r="L2" s="44" t="s">
         <v>302</v>
-      </c>
-      <c r="L2" s="44" t="s">
-        <v>303</v>
       </c>
       <c r="M2" s="44">
         <v>2</v>
       </c>
       <c r="N2" s="44" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="14.4" thickBot="1">
@@ -8040,43 +8040,43 @@
         <v>252</v>
       </c>
       <c r="B3" s="44" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C3" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D3" s="44" t="s">
+        <v>334</v>
+      </c>
+      <c r="E3" s="44" t="s">
+        <v>505</v>
+      </c>
+      <c r="F3" s="44" t="s">
         <v>335</v>
       </c>
-      <c r="E3" s="44" t="s">
-        <v>506</v>
-      </c>
-      <c r="F3" s="44" t="s">
+      <c r="G3" s="44" t="s">
+        <v>298</v>
+      </c>
+      <c r="H3" s="44" t="s">
+        <v>335</v>
+      </c>
+      <c r="I3" s="44" t="s">
         <v>336</v>
       </c>
-      <c r="G3" s="44" t="s">
-        <v>299</v>
-      </c>
-      <c r="H3" s="44" t="s">
-        <v>336</v>
-      </c>
-      <c r="I3" s="44" t="s">
+      <c r="J3" s="44" t="s">
+        <v>300</v>
+      </c>
+      <c r="K3" s="44" t="s">
+        <v>301</v>
+      </c>
+      <c r="L3" s="44" t="s">
         <v>337</v>
-      </c>
-      <c r="J3" s="44" t="s">
-        <v>301</v>
-      </c>
-      <c r="K3" s="44" t="s">
-        <v>302</v>
-      </c>
-      <c r="L3" s="44" t="s">
-        <v>338</v>
       </c>
       <c r="M3" s="44">
         <v>1</v>
       </c>
       <c r="N3" s="44" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="28.2" thickBot="1">
@@ -8084,43 +8084,43 @@
         <v>252</v>
       </c>
       <c r="B4" s="44" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C4" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D4" s="44" t="s">
+        <v>338</v>
+      </c>
+      <c r="E4" s="44" t="s">
+        <v>505</v>
+      </c>
+      <c r="F4" s="44" t="s">
         <v>339</v>
       </c>
-      <c r="E4" s="44" t="s">
-        <v>506</v>
-      </c>
-      <c r="F4" s="44" t="s">
+      <c r="G4" s="44" t="s">
+        <v>321</v>
+      </c>
+      <c r="H4" s="44" t="s">
+        <v>339</v>
+      </c>
+      <c r="I4" s="44" t="s">
         <v>340</v>
       </c>
-      <c r="G4" s="44" t="s">
-        <v>322</v>
-      </c>
-      <c r="H4" s="44" t="s">
-        <v>340</v>
-      </c>
-      <c r="I4" s="44" t="s">
+      <c r="J4" s="44" t="s">
+        <v>300</v>
+      </c>
+      <c r="K4" s="44" t="s">
+        <v>301</v>
+      </c>
+      <c r="L4" s="44" t="s">
         <v>341</v>
-      </c>
-      <c r="J4" s="44" t="s">
-        <v>301</v>
-      </c>
-      <c r="K4" s="44" t="s">
-        <v>302</v>
-      </c>
-      <c r="L4" s="44" t="s">
-        <v>342</v>
       </c>
       <c r="M4" s="44">
         <v>2</v>
       </c>
       <c r="N4" s="44" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="28.2" thickBot="1">
@@ -8128,43 +8128,43 @@
         <v>252</v>
       </c>
       <c r="B5" s="44" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C5" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D5" s="44" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E5" s="44" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="F5" s="44" t="s">
         <v>252</v>
       </c>
       <c r="G5" s="44" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="H5" s="44" t="s">
         <v>252</v>
       </c>
       <c r="I5" s="44" t="s">
+        <v>343</v>
+      </c>
+      <c r="J5" s="44" t="s">
+        <v>316</v>
+      </c>
+      <c r="K5" s="44" t="s">
+        <v>317</v>
+      </c>
+      <c r="L5" s="44" t="s">
         <v>344</v>
-      </c>
-      <c r="J5" s="44" t="s">
-        <v>317</v>
-      </c>
-      <c r="K5" s="44" t="s">
-        <v>318</v>
-      </c>
-      <c r="L5" s="44" t="s">
-        <v>345</v>
       </c>
       <c r="M5" s="44">
         <v>1</v>
       </c>
       <c r="N5" s="44" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="42" thickBot="1">
@@ -8172,43 +8172,43 @@
         <v>260</v>
       </c>
       <c r="B6" s="44" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C6" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D6" s="44" t="s">
+        <v>306</v>
+      </c>
+      <c r="E6" s="44" t="s">
+        <v>505</v>
+      </c>
+      <c r="F6" s="44" t="s">
         <v>307</v>
       </c>
-      <c r="E6" s="44" t="s">
-        <v>506</v>
-      </c>
-      <c r="F6" s="44" t="s">
+      <c r="G6" s="44" t="s">
+        <v>298</v>
+      </c>
+      <c r="H6" s="44" t="s">
+        <v>307</v>
+      </c>
+      <c r="I6" s="44" t="s">
         <v>308</v>
       </c>
-      <c r="G6" s="44" t="s">
-        <v>299</v>
-      </c>
-      <c r="H6" s="44" t="s">
-        <v>308</v>
-      </c>
-      <c r="I6" s="44" t="s">
+      <c r="J6" s="44" t="s">
+        <v>300</v>
+      </c>
+      <c r="K6" s="44" t="s">
+        <v>301</v>
+      </c>
+      <c r="L6" s="44" t="s">
         <v>309</v>
-      </c>
-      <c r="J6" s="44" t="s">
-        <v>301</v>
-      </c>
-      <c r="K6" s="44" t="s">
-        <v>302</v>
-      </c>
-      <c r="L6" s="44" t="s">
-        <v>310</v>
       </c>
       <c r="M6" s="44">
         <v>2</v>
       </c>
       <c r="N6" s="44" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="14.4" thickBot="1">
@@ -8216,43 +8216,43 @@
         <v>260</v>
       </c>
       <c r="B7" s="44" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D7" s="44" t="s">
+        <v>345</v>
+      </c>
+      <c r="E7" s="44" t="s">
+        <v>505</v>
+      </c>
+      <c r="F7" s="44" t="s">
         <v>346</v>
       </c>
-      <c r="E7" s="44" t="s">
-        <v>506</v>
-      </c>
-      <c r="F7" s="44" t="s">
+      <c r="G7" s="44" t="s">
         <v>347</v>
       </c>
-      <c r="G7" s="44" t="s">
+      <c r="H7" s="44" t="s">
+        <v>346</v>
+      </c>
+      <c r="I7" s="44" t="s">
         <v>348</v>
       </c>
-      <c r="H7" s="44" t="s">
-        <v>347</v>
-      </c>
-      <c r="I7" s="44" t="s">
+      <c r="J7" s="44" t="s">
+        <v>316</v>
+      </c>
+      <c r="K7" s="44" t="s">
+        <v>317</v>
+      </c>
+      <c r="L7" s="44" t="s">
         <v>349</v>
-      </c>
-      <c r="J7" s="44" t="s">
-        <v>317</v>
-      </c>
-      <c r="K7" s="44" t="s">
-        <v>318</v>
-      </c>
-      <c r="L7" s="44" t="s">
-        <v>350</v>
       </c>
       <c r="M7" s="44">
         <v>1</v>
       </c>
       <c r="N7" s="44" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="28.2" thickBot="1">
@@ -8260,43 +8260,43 @@
         <v>269</v>
       </c>
       <c r="B8" s="44" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C8" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D8" s="44" t="s">
+        <v>312</v>
+      </c>
+      <c r="E8" s="44" t="s">
+        <v>505</v>
+      </c>
+      <c r="F8" s="44" t="s">
         <v>313</v>
       </c>
-      <c r="E8" s="44" t="s">
-        <v>506</v>
-      </c>
-      <c r="F8" s="44" t="s">
+      <c r="G8" s="44" t="s">
         <v>314</v>
       </c>
-      <c r="G8" s="44" t="s">
+      <c r="H8" s="44" t="s">
+        <v>313</v>
+      </c>
+      <c r="I8" s="44" t="s">
         <v>315</v>
       </c>
-      <c r="H8" s="44" t="s">
-        <v>314</v>
-      </c>
-      <c r="I8" s="44" t="s">
+      <c r="J8" s="44" t="s">
         <v>316</v>
       </c>
-      <c r="J8" s="44" t="s">
+      <c r="K8" s="44" t="s">
         <v>317</v>
       </c>
-      <c r="K8" s="44" t="s">
+      <c r="L8" s="44" t="s">
         <v>318</v>
-      </c>
-      <c r="L8" s="44" t="s">
-        <v>319</v>
       </c>
       <c r="M8" s="44">
         <v>2</v>
       </c>
       <c r="N8" s="44" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="28.2" thickBot="1">
@@ -8304,43 +8304,43 @@
         <v>269</v>
       </c>
       <c r="B9" s="44" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C9" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D9" s="44" t="s">
+        <v>350</v>
+      </c>
+      <c r="E9" s="44" t="s">
+        <v>505</v>
+      </c>
+      <c r="F9" s="44" t="s">
         <v>351</v>
       </c>
-      <c r="E9" s="44" t="s">
-        <v>506</v>
-      </c>
-      <c r="F9" s="44" t="s">
+      <c r="G9" s="44" t="s">
+        <v>310</v>
+      </c>
+      <c r="H9" s="44" t="s">
+        <v>351</v>
+      </c>
+      <c r="I9" s="44" t="s">
         <v>352</v>
       </c>
-      <c r="G9" s="44" t="s">
-        <v>311</v>
-      </c>
-      <c r="H9" s="44" t="s">
-        <v>352</v>
-      </c>
-      <c r="I9" s="44" t="s">
+      <c r="J9" s="44" t="s">
+        <v>304</v>
+      </c>
+      <c r="K9" s="44" t="s">
+        <v>305</v>
+      </c>
+      <c r="L9" s="44" t="s">
         <v>353</v>
-      </c>
-      <c r="J9" s="44" t="s">
-        <v>305</v>
-      </c>
-      <c r="K9" s="44" t="s">
-        <v>306</v>
-      </c>
-      <c r="L9" s="44" t="s">
-        <v>354</v>
       </c>
       <c r="M9" s="44">
         <v>1</v>
       </c>
       <c r="N9" s="44" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="28.2" thickBot="1">
@@ -8348,43 +8348,43 @@
         <v>269</v>
       </c>
       <c r="B10" s="44" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C10" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D10" s="44" t="s">
+        <v>354</v>
+      </c>
+      <c r="E10" s="44" t="s">
+        <v>505</v>
+      </c>
+      <c r="F10" s="44" t="s">
         <v>355</v>
       </c>
-      <c r="E10" s="44" t="s">
-        <v>506</v>
-      </c>
-      <c r="F10" s="44" t="s">
+      <c r="G10" s="44" t="s">
+        <v>310</v>
+      </c>
+      <c r="H10" s="44" t="s">
+        <v>355</v>
+      </c>
+      <c r="I10" s="44" t="s">
         <v>356</v>
       </c>
-      <c r="G10" s="44" t="s">
-        <v>311</v>
-      </c>
-      <c r="H10" s="44" t="s">
-        <v>356</v>
-      </c>
-      <c r="I10" s="44" t="s">
+      <c r="J10" s="44" t="s">
+        <v>316</v>
+      </c>
+      <c r="K10" s="44" t="s">
+        <v>317</v>
+      </c>
+      <c r="L10" s="44" t="s">
         <v>357</v>
-      </c>
-      <c r="J10" s="44" t="s">
-        <v>317</v>
-      </c>
-      <c r="K10" s="44" t="s">
-        <v>318</v>
-      </c>
-      <c r="L10" s="44" t="s">
-        <v>358</v>
       </c>
       <c r="M10" s="44">
         <v>1</v>
       </c>
       <c r="N10" s="44" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="28.2" thickBot="1">
@@ -8392,43 +8392,43 @@
         <v>269</v>
       </c>
       <c r="B11" s="44" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C11" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D11" s="44" t="s">
+        <v>358</v>
+      </c>
+      <c r="E11" s="44" t="s">
+        <v>505</v>
+      </c>
+      <c r="F11" s="44" t="s">
         <v>359</v>
       </c>
-      <c r="E11" s="44" t="s">
-        <v>506</v>
-      </c>
-      <c r="F11" s="44" t="s">
+      <c r="G11" s="44" t="s">
         <v>360</v>
       </c>
-      <c r="G11" s="44" t="s">
+      <c r="H11" s="44" t="s">
+        <v>359</v>
+      </c>
+      <c r="I11" s="44" t="s">
         <v>361</v>
       </c>
-      <c r="H11" s="44" t="s">
-        <v>360</v>
-      </c>
-      <c r="I11" s="44" t="s">
+      <c r="J11" s="44" t="s">
+        <v>304</v>
+      </c>
+      <c r="K11" s="44" t="s">
+        <v>305</v>
+      </c>
+      <c r="L11" s="44" t="s">
         <v>362</v>
-      </c>
-      <c r="J11" s="44" t="s">
-        <v>305</v>
-      </c>
-      <c r="K11" s="44" t="s">
-        <v>306</v>
-      </c>
-      <c r="L11" s="44" t="s">
-        <v>363</v>
       </c>
       <c r="M11" s="44">
         <v>1</v>
       </c>
       <c r="N11" s="44" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="28.2" thickBot="1">
@@ -8436,43 +8436,43 @@
         <v>277</v>
       </c>
       <c r="B12" s="44" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C12" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D12" s="44" t="s">
+        <v>319</v>
+      </c>
+      <c r="E12" s="44" t="s">
+        <v>505</v>
+      </c>
+      <c r="F12" s="44" t="s">
         <v>320</v>
       </c>
-      <c r="E12" s="44" t="s">
-        <v>506</v>
-      </c>
-      <c r="F12" s="44" t="s">
+      <c r="G12" s="44" t="s">
         <v>321</v>
       </c>
-      <c r="G12" s="44" t="s">
+      <c r="H12" s="44" t="s">
+        <v>320</v>
+      </c>
+      <c r="I12" s="44" t="s">
         <v>322</v>
       </c>
-      <c r="H12" s="44" t="s">
-        <v>321</v>
-      </c>
-      <c r="I12" s="44" t="s">
+      <c r="J12" s="44" t="s">
+        <v>300</v>
+      </c>
+      <c r="K12" s="44" t="s">
+        <v>301</v>
+      </c>
+      <c r="L12" s="44" t="s">
         <v>323</v>
-      </c>
-      <c r="J12" s="44" t="s">
-        <v>301</v>
-      </c>
-      <c r="K12" s="44" t="s">
-        <v>302</v>
-      </c>
-      <c r="L12" s="44" t="s">
-        <v>324</v>
       </c>
       <c r="M12" s="44">
         <v>2</v>
       </c>
       <c r="N12" s="44" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="28.2" thickBot="1">
@@ -8480,131 +8480,131 @@
         <v>277</v>
       </c>
       <c r="B13" s="44" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C13" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D13" s="44" t="s">
+        <v>363</v>
+      </c>
+      <c r="E13" s="44" t="s">
+        <v>505</v>
+      </c>
+      <c r="F13" s="44" t="s">
         <v>364</v>
       </c>
-      <c r="E13" s="44" t="s">
-        <v>506</v>
-      </c>
-      <c r="F13" s="44" t="s">
+      <c r="G13" s="44" t="s">
+        <v>324</v>
+      </c>
+      <c r="H13" s="44" t="s">
+        <v>364</v>
+      </c>
+      <c r="I13" s="44" t="s">
         <v>365</v>
       </c>
-      <c r="G13" s="44" t="s">
-        <v>325</v>
-      </c>
-      <c r="H13" s="44" t="s">
-        <v>365</v>
-      </c>
-      <c r="I13" s="44" t="s">
+      <c r="J13" s="44" t="s">
+        <v>316</v>
+      </c>
+      <c r="K13" s="44" t="s">
+        <v>317</v>
+      </c>
+      <c r="L13" s="44" t="s">
         <v>366</v>
-      </c>
-      <c r="J13" s="44" t="s">
-        <v>317</v>
-      </c>
-      <c r="K13" s="44" t="s">
-        <v>318</v>
-      </c>
-      <c r="L13" s="44" t="s">
-        <v>367</v>
       </c>
       <c r="M13" s="44">
         <v>1</v>
       </c>
       <c r="N13" s="44" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="14.4" thickBot="1">
       <c r="A14" s="44" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B14" s="44" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C14" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D14" s="44" t="s">
+        <v>325</v>
+      </c>
+      <c r="E14" s="44" t="s">
+        <v>505</v>
+      </c>
+      <c r="F14" s="44" t="s">
         <v>326</v>
       </c>
-      <c r="E14" s="44" t="s">
-        <v>506</v>
-      </c>
-      <c r="F14" s="44" t="s">
+      <c r="G14" s="44" t="s">
         <v>327</v>
       </c>
-      <c r="G14" s="44" t="s">
+      <c r="H14" s="44" t="s">
+        <v>326</v>
+      </c>
+      <c r="I14" s="44" t="s">
         <v>328</v>
       </c>
-      <c r="H14" s="44" t="s">
-        <v>327</v>
-      </c>
-      <c r="I14" s="44" t="s">
+      <c r="J14" s="44" t="s">
+        <v>316</v>
+      </c>
+      <c r="K14" s="44" t="s">
+        <v>317</v>
+      </c>
+      <c r="L14" s="44" t="s">
         <v>329</v>
-      </c>
-      <c r="J14" s="44" t="s">
-        <v>317</v>
-      </c>
-      <c r="K14" s="44" t="s">
-        <v>318</v>
-      </c>
-      <c r="L14" s="44" t="s">
-        <v>330</v>
       </c>
       <c r="M14" s="44">
         <v>2</v>
       </c>
       <c r="N14" s="44" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="28.2" thickBot="1">
       <c r="A15" s="44" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B15" s="44" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C15" s="44" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D15" s="44" t="s">
+        <v>367</v>
+      </c>
+      <c r="E15" s="44" t="s">
+        <v>505</v>
+      </c>
+      <c r="F15" s="44" t="s">
         <v>368</v>
       </c>
-      <c r="E15" s="44" t="s">
-        <v>506</v>
-      </c>
-      <c r="F15" s="44" t="s">
+      <c r="G15" s="44" t="s">
+        <v>330</v>
+      </c>
+      <c r="H15" s="44" t="s">
+        <v>368</v>
+      </c>
+      <c r="I15" s="44" t="s">
         <v>369</v>
       </c>
-      <c r="G15" s="44" t="s">
-        <v>331</v>
-      </c>
-      <c r="H15" s="44" t="s">
-        <v>369</v>
-      </c>
-      <c r="I15" s="44" t="s">
+      <c r="J15" s="44" t="s">
+        <v>304</v>
+      </c>
+      <c r="K15" s="44" t="s">
+        <v>305</v>
+      </c>
+      <c r="L15" s="44" t="s">
         <v>370</v>
-      </c>
-      <c r="J15" s="44" t="s">
-        <v>305</v>
-      </c>
-      <c r="K15" s="44" t="s">
-        <v>306</v>
-      </c>
-      <c r="L15" s="44" t="s">
-        <v>371</v>
       </c>
       <c r="M15" s="44">
         <v>1</v>
       </c>
       <c r="N15" s="44" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -8632,7 +8632,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15" thickBot="1">
       <c r="A1" s="32" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B1" s="46" t="s">
         <v>59</v>
@@ -8644,313 +8644,313 @@
         <v>61</v>
       </c>
       <c r="E1" s="34" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" thickBot="1">
       <c r="A2" s="44" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B2" s="44" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C2" s="44" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D2" s="44" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="E2" s="44" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" thickBot="1">
       <c r="A3" s="44" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B3" s="44" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C3" s="44" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D3" s="44" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="E3" s="44" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" thickBot="1">
       <c r="A4" s="44" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B4" s="44" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C4" s="44" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D4" s="44" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="E4" s="44" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1">
       <c r="A5" s="44" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B5" s="44" t="s">
+        <v>612</v>
+      </c>
+      <c r="C5" s="44" t="s">
+        <v>373</v>
+      </c>
+      <c r="D5" s="44" t="s">
         <v>613</v>
       </c>
-      <c r="C5" s="44" t="s">
-        <v>374</v>
-      </c>
-      <c r="D5" s="44" t="s">
-        <v>614</v>
-      </c>
       <c r="E5" s="44" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" thickBot="1">
       <c r="A6" s="44" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B6" s="44" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C6" s="44" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D6" s="44" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="E6" s="44" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" thickBot="1">
       <c r="A7" s="44" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B7" s="44" t="s">
+        <v>612</v>
+      </c>
+      <c r="C7" s="44" t="s">
+        <v>332</v>
+      </c>
+      <c r="D7" s="44" t="s">
         <v>613</v>
       </c>
-      <c r="C7" s="44" t="s">
-        <v>333</v>
-      </c>
-      <c r="D7" s="44" t="s">
-        <v>614</v>
-      </c>
       <c r="E7" s="44" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="28.2" thickBot="1">
       <c r="A8" s="44" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B8" s="44" t="s">
+        <v>614</v>
+      </c>
+      <c r="C8" s="44" t="s">
+        <v>374</v>
+      </c>
+      <c r="D8" s="44" t="s">
         <v>615</v>
       </c>
-      <c r="C8" s="44" t="s">
-        <v>375</v>
-      </c>
-      <c r="D8" s="44" t="s">
-        <v>616</v>
-      </c>
       <c r="E8" s="44" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" thickBot="1">
       <c r="A9" s="44" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B9" s="44" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C9" s="44" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D9" s="44" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="E9" s="44" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" thickBot="1">
       <c r="A10" s="44" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B10" s="44" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C10" s="44" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D10" s="44" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="E10" s="44" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="28.2" thickBot="1">
       <c r="A11" s="44" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B11" s="44" t="s">
+        <v>614</v>
+      </c>
+      <c r="C11" s="44" t="s">
+        <v>331</v>
+      </c>
+      <c r="D11" s="44" t="s">
         <v>615</v>
       </c>
-      <c r="C11" s="44" t="s">
-        <v>332</v>
-      </c>
-      <c r="D11" s="44" t="s">
-        <v>616</v>
-      </c>
       <c r="E11" s="44" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15" thickBot="1">
       <c r="A12" s="44" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B12" s="44" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C12" s="44" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D12" s="44" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="E12" s="44" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15" thickBot="1">
       <c r="A13" s="44" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B13" s="44" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="C13" s="44" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D13" s="44" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="E13" s="44" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15" thickBot="1">
       <c r="A14" s="44" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B14" s="44" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="C14" s="44" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D14" s="44" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="E14" s="44" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="28.2" thickBot="1">
       <c r="A15" s="44" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B15" s="44" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="C15" s="44" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D15" s="44" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="E15" s="44" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15" thickBot="1">
       <c r="A16" s="44" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B16" s="44" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C16" s="44" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D16" s="44" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="E16" s="44" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15" thickBot="1">
       <c r="A17" s="44" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B17" s="44" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C17" s="44" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D17" s="44" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="E17" s="44" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" thickBot="1">
       <c r="A18" s="44" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B18" s="44" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C18" s="44" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D18" s="44" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="E18" s="44" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15" thickBot="1">
       <c r="A19" s="44" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B19" s="44" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C19" s="44" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D19" s="44" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="E19" s="44" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
   </sheetData>
@@ -8963,7 +8963,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D72D8E99-EB27-4476-B552-FC62C760077E}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="A1:B5"/>
     </sheetView>
   </sheetViews>
@@ -8979,39 +8979,39 @@
         <v>251</v>
       </c>
       <c r="B1" s="57" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14.4">
       <c r="A2" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B2" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="14.4">
       <c r="A3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B3" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.4">
       <c r="A4" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B4" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="14.4">
       <c r="A5" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B5" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
   </sheetData>
@@ -9039,67 +9039,67 @@
         <v>251</v>
       </c>
       <c r="B1" s="51" t="s">
+        <v>511</v>
+      </c>
+      <c r="C1" s="51" t="s">
+        <v>543</v>
+      </c>
+      <c r="D1" s="51" t="s">
+        <v>544</v>
+      </c>
+      <c r="E1" s="51" t="s">
         <v>512</v>
-      </c>
-      <c r="C1" s="51" t="s">
-        <v>544</v>
-      </c>
-      <c r="D1" s="51" t="s">
-        <v>545</v>
-      </c>
-      <c r="E1" s="51" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1">
       <c r="A2" s="44" t="s">
+        <v>526</v>
+      </c>
+      <c r="B2" s="44" t="s">
         <v>527</v>
       </c>
-      <c r="B2" s="44" t="s">
-        <v>528</v>
-      </c>
       <c r="C2" s="44" t="s">
+        <v>601</v>
+      </c>
+      <c r="D2" s="44" t="s">
+        <v>546</v>
+      </c>
+      <c r="E2" s="44" t="s">
         <v>602</v>
-      </c>
-      <c r="D2" s="44" t="s">
-        <v>547</v>
-      </c>
-      <c r="E2" s="44" t="s">
-        <v>603</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1">
       <c r="A3" s="50" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B3" s="50" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C3" s="50" t="s">
+        <v>545</v>
+      </c>
+      <c r="D3" s="50" t="s">
         <v>546</v>
       </c>
-      <c r="D3" s="50" t="s">
+      <c r="E3" s="50" t="s">
         <v>547</v>
-      </c>
-      <c r="E3" s="50" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1">
       <c r="A4" s="44" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B4" s="44" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C4" s="44" t="s">
+        <v>548</v>
+      </c>
+      <c r="D4" s="44" t="s">
+        <v>546</v>
+      </c>
+      <c r="E4" s="44" t="s">
         <v>549</v>
-      </c>
-      <c r="D4" s="44" t="s">
-        <v>547</v>
-      </c>
-      <c r="E4" s="44" t="s">
-        <v>550</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1">
@@ -9110,98 +9110,98 @@
         <v>91</v>
       </c>
       <c r="C5" s="44" t="s">
+        <v>550</v>
+      </c>
+      <c r="D5" s="44" t="s">
         <v>551</v>
       </c>
-      <c r="D5" s="44" t="s">
+      <c r="E5" s="44" t="s">
         <v>552</v>
-      </c>
-      <c r="E5" s="44" t="s">
-        <v>553</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1">
       <c r="A6" s="44" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B6" s="44" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C6" s="44" t="s">
+        <v>553</v>
+      </c>
+      <c r="D6" s="44" t="s">
         <v>554</v>
       </c>
-      <c r="D6" s="44" t="s">
+      <c r="E6" s="44" t="s">
         <v>555</v>
-      </c>
-      <c r="E6" s="44" t="s">
-        <v>556</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1">
       <c r="A7" s="44" t="s">
+        <v>524</v>
+      </c>
+      <c r="B7" s="44" t="s">
         <v>525</v>
       </c>
-      <c r="B7" s="44" t="s">
-        <v>526</v>
-      </c>
       <c r="C7" s="44" t="s">
+        <v>561</v>
+      </c>
+      <c r="D7" s="44" t="s">
         <v>562</v>
       </c>
-      <c r="D7" s="44" t="s">
-        <v>563</v>
-      </c>
       <c r="E7" s="44" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1">
       <c r="A8" s="44" t="s">
+        <v>522</v>
+      </c>
+      <c r="B8" s="44" t="s">
         <v>523</v>
       </c>
-      <c r="B8" s="44" t="s">
-        <v>524</v>
-      </c>
       <c r="C8" s="44" t="s">
+        <v>561</v>
+      </c>
+      <c r="D8" s="44" t="s">
         <v>562</v>
       </c>
-      <c r="D8" s="44" t="s">
+      <c r="E8" s="44" t="s">
         <v>563</v>
-      </c>
-      <c r="E8" s="44" t="s">
-        <v>564</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1">
       <c r="A9" s="44" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B9" s="44" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C9" s="44" t="s">
+        <v>559</v>
+      </c>
+      <c r="D9" s="54" t="s">
+        <v>557</v>
+      </c>
+      <c r="E9" s="44" t="s">
         <v>560</v>
-      </c>
-      <c r="D9" s="54" t="s">
-        <v>558</v>
-      </c>
-      <c r="E9" s="44" t="s">
-        <v>561</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1">
       <c r="A10" s="44" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B10" s="44" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C10" s="52" t="s">
+        <v>556</v>
+      </c>
+      <c r="D10" s="55" t="s">
         <v>557</v>
       </c>
-      <c r="D10" s="55" t="s">
+      <c r="E10" s="53" t="s">
         <v>558</v>
-      </c>
-      <c r="E10" s="53" t="s">
-        <v>559</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1">
@@ -9212,234 +9212,234 @@
         <v>65</v>
       </c>
       <c r="C11" s="44" t="s">
+        <v>565</v>
+      </c>
+      <c r="D11" s="50" t="s">
         <v>566</v>
       </c>
-      <c r="D11" s="50" t="s">
+      <c r="E11" s="44" t="s">
         <v>567</v>
-      </c>
-      <c r="E11" s="44" t="s">
-        <v>568</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1">
       <c r="A12" s="44" t="s">
+        <v>540</v>
+      </c>
+      <c r="B12" s="44" t="s">
         <v>541</v>
       </c>
-      <c r="B12" s="44" t="s">
-        <v>542</v>
-      </c>
       <c r="C12" s="44" t="s">
+        <v>568</v>
+      </c>
+      <c r="D12" s="44" t="s">
         <v>569</v>
       </c>
-      <c r="D12" s="44" t="s">
+      <c r="E12" s="44" t="s">
         <v>570</v>
-      </c>
-      <c r="E12" s="44" t="s">
-        <v>571</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1">
       <c r="A13" s="44" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B13" s="44" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C13" s="44" t="s">
+        <v>571</v>
+      </c>
+      <c r="D13" s="44" t="s">
         <v>572</v>
       </c>
-      <c r="D13" s="44" t="s">
+      <c r="E13" s="44" t="s">
         <v>573</v>
-      </c>
-      <c r="E13" s="44" t="s">
-        <v>574</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1">
       <c r="A14" s="44" t="s">
+        <v>534</v>
+      </c>
+      <c r="B14" s="44" t="s">
         <v>535</v>
       </c>
-      <c r="B14" s="44" t="s">
-        <v>536</v>
-      </c>
       <c r="C14" s="44" t="s">
+        <v>574</v>
+      </c>
+      <c r="D14" s="44" t="s">
         <v>575</v>
       </c>
-      <c r="D14" s="44" t="s">
+      <c r="E14" s="44" t="s">
         <v>576</v>
-      </c>
-      <c r="E14" s="44" t="s">
-        <v>577</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1">
       <c r="A15" s="44" t="s">
+        <v>536</v>
+      </c>
+      <c r="B15" s="44" t="s">
         <v>537</v>
       </c>
-      <c r="B15" s="44" t="s">
-        <v>538</v>
-      </c>
       <c r="C15" s="44" t="s">
+        <v>577</v>
+      </c>
+      <c r="D15" s="44" t="s">
         <v>578</v>
       </c>
-      <c r="D15" s="44" t="s">
+      <c r="E15" s="44" t="s">
         <v>579</v>
-      </c>
-      <c r="E15" s="44" t="s">
-        <v>580</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1">
       <c r="A16" s="44" t="s">
+        <v>538</v>
+      </c>
+      <c r="B16" s="44" t="s">
         <v>539</v>
       </c>
-      <c r="B16" s="44" t="s">
-        <v>540</v>
-      </c>
       <c r="C16" s="44" t="s">
+        <v>580</v>
+      </c>
+      <c r="D16" s="44" t="s">
         <v>581</v>
       </c>
-      <c r="D16" s="44" t="s">
+      <c r="E16" s="44" t="s">
         <v>582</v>
-      </c>
-      <c r="E16" s="44" t="s">
-        <v>583</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1">
       <c r="A17" s="44" t="s">
+        <v>528</v>
+      </c>
+      <c r="B17" s="44" t="s">
         <v>529</v>
       </c>
-      <c r="B17" s="44" t="s">
-        <v>530</v>
-      </c>
       <c r="C17" s="44" t="s">
+        <v>583</v>
+      </c>
+      <c r="D17" s="44" t="s">
         <v>584</v>
       </c>
-      <c r="D17" s="44" t="s">
+      <c r="E17" s="44" t="s">
         <v>585</v>
-      </c>
-      <c r="E17" s="44" t="s">
-        <v>586</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1">
       <c r="A18" s="44" t="s">
+        <v>516</v>
+      </c>
+      <c r="B18" s="44" t="s">
         <v>517</v>
       </c>
-      <c r="B18" s="44" t="s">
-        <v>518</v>
-      </c>
       <c r="C18" s="44" t="s">
+        <v>586</v>
+      </c>
+      <c r="D18" s="44" t="s">
         <v>587</v>
       </c>
-      <c r="D18" s="44" t="s">
+      <c r="E18" s="44" t="s">
         <v>588</v>
-      </c>
-      <c r="E18" s="44" t="s">
-        <v>589</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1">
       <c r="A19" s="44" t="s">
+        <v>532</v>
+      </c>
+      <c r="B19" s="44" t="s">
         <v>533</v>
       </c>
-      <c r="B19" s="44" t="s">
-        <v>534</v>
-      </c>
       <c r="C19" s="44" t="s">
+        <v>589</v>
+      </c>
+      <c r="D19" s="44" t="s">
         <v>590</v>
       </c>
-      <c r="D19" s="44" t="s">
+      <c r="E19" s="44" t="s">
         <v>591</v>
-      </c>
-      <c r="E19" s="44" t="s">
-        <v>592</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1">
       <c r="A20" s="44" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B20" s="44" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C20" s="44" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="D20" s="44" t="s">
+        <v>592</v>
+      </c>
+      <c r="E20" s="44" t="s">
         <v>593</v>
-      </c>
-      <c r="E20" s="44" t="s">
-        <v>594</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1">
       <c r="A21" s="44" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B21" s="44" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C21" s="44" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="D21" s="44" t="s">
+        <v>594</v>
+      </c>
+      <c r="E21" s="44" t="s">
         <v>595</v>
-      </c>
-      <c r="E21" s="44" t="s">
-        <v>596</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1">
       <c r="A22" s="44" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B22" s="44" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C22" s="44" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D22" s="44" t="s">
+        <v>596</v>
+      </c>
+      <c r="E22" s="44" t="s">
         <v>597</v>
-      </c>
-      <c r="E22" s="44" t="s">
-        <v>598</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1">
       <c r="A23" s="44" t="s">
+        <v>513</v>
+      </c>
+      <c r="B23" s="44" t="s">
         <v>514</v>
       </c>
-      <c r="B23" s="44" t="s">
-        <v>515</v>
-      </c>
       <c r="C23" s="44" t="s">
+        <v>598</v>
+      </c>
+      <c r="D23" s="44" t="s">
         <v>599</v>
       </c>
-      <c r="D23" s="44" t="s">
+      <c r="E23" s="44" t="s">
         <v>600</v>
-      </c>
-      <c r="E23" s="44" t="s">
-        <v>601</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="18.600000000000001" customHeight="1" thickBot="1">
       <c r="A24" s="44" t="s">
+        <v>530</v>
+      </c>
+      <c r="B24" s="44" t="s">
         <v>531</v>
       </c>
-      <c r="B24" s="44" t="s">
-        <v>532</v>
-      </c>
       <c r="C24" s="44" t="s">
+        <v>603</v>
+      </c>
+      <c r="D24" s="44" t="s">
         <v>604</v>
       </c>
-      <c r="D24" s="44" t="s">
+      <c r="E24" s="44" t="s">
         <v>605</v>
-      </c>
-      <c r="E24" s="44" t="s">
-        <v>606</v>
       </c>
     </row>
   </sheetData>
@@ -9448,26 +9448,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3313e3b7-7be6-4700-b36c-ef100101b814">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="92fd223e-acad-439f-bdfb-a3d2d2c3e354" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001823FE8F7B9D0E4D8E2A8BCA9CE24B29" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="73c723fc07ccc7486cedfbfb910c1aef">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3313e3b7-7be6-4700-b36c-ef100101b814" xmlns:ns3="92fd223e-acad-439f-bdfb-a3d2d2c3e354" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="53ff358aed99a442890d21eb5fffdaa6" ns2:_="" ns3:_="">
     <xsd:import namespace="3313e3b7-7be6-4700-b36c-ef100101b814"/>
@@ -9702,10 +9682,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3313e3b7-7be6-4700-b36c-ef100101b814">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="92fd223e-acad-439f-bdfb-a3d2d2c3e354" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9AD11F7-4AE8-4103-B6AA-C2660A052287}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC33D7E9-29AE-406E-91EA-76B3A0E344D1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3313e3b7-7be6-4700-b36c-ef100101b814"/>
+    <ds:schemaRef ds:uri="92fd223e-acad-439f-bdfb-a3d2d2c3e354"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9728,20 +9739,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC33D7E9-29AE-406E-91EA-76B3A0E344D1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9AD11F7-4AE8-4103-B6AA-C2660A052287}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="3313e3b7-7be6-4700-b36c-ef100101b814"/>
-    <ds:schemaRef ds:uri="92fd223e-acad-439f-bdfb-a3d2d2c3e354"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>